<commit_message>
Add updated Data Cleaning and Excel Charts tutorial files; include new Excel Project Dataset
</commit_message>
<xml_diff>
--- a/Excel/Data Cleaning Excel Tutorial.xlsx
+++ b/Excel/Data Cleaning Excel Tutorial.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/579481080490e445/Documents/Excel Series Excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\sql_practice\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{C3F4832D-6691-4E80-9CE5-51C600B1F941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF1BDEA-BCC1-43F9-93D7-324A2E9B60D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="14586" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="US_Presidents Excel Tutorial Da" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'US_Presidents Excel Tutorial Da'!$A$1:$H$48</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="94">
   <si>
     <t>S.No.</t>
   </si>
@@ -40,99 +43,39 @@
     <t>president</t>
   </si>
   <si>
-    <t>prior</t>
-  </si>
-  <si>
     <t>party</t>
   </si>
   <si>
     <t>vice</t>
   </si>
   <si>
-    <t>George Washington</t>
-  </si>
-  <si>
-    <t>Commander-in-Chief  of the  Continental Army   ( 1775â€“1783 )</t>
-  </si>
-  <si>
     <t>John Adams</t>
   </si>
   <si>
     <t>john adams</t>
   </si>
   <si>
-    <t>1st  Vice President of the United States</t>
-  </si>
-  <si>
     <t>Federalist</t>
   </si>
   <si>
     <t>Thomas Jefferson</t>
   </si>
   <si>
-    <t>2nd  Vice President of the United States</t>
-  </si>
-  <si>
     <t>Democratic-  Republican</t>
   </si>
   <si>
-    <t xml:space="preserve">    Aaron Burr</t>
-  </si>
-  <si>
-    <t>James Madison</t>
-  </si>
-  <si>
-    <t>5th  United States Secretary of State   (1801â€“1809)</t>
-  </si>
-  <si>
-    <t>George    Clinton</t>
-  </si>
-  <si>
-    <t>JAMES MONROE</t>
-  </si>
-  <si>
-    <t>7th  United States Secretary of State   (1811â€“1817)</t>
-  </si>
-  <si>
     <t>Daniel D. Tompkins</t>
   </si>
   <si>
-    <t>John Quincy Adams</t>
-  </si>
-  <si>
-    <t>8th  United States Secretary of State   (1817â€“1825)</t>
-  </si>
-  <si>
     <t>John C. Calhoun</t>
   </si>
   <si>
-    <t>Andrew Jackson</t>
-  </si>
-  <si>
-    <t>U.S. Senator   ( Class 2 )   from  Tennessee   (1823â€“1825)</t>
-  </si>
-  <si>
     <t>Democratic</t>
   </si>
   <si>
-    <t>John C.     Calhoun</t>
-  </si>
-  <si>
-    <t>Martin Van Buren</t>
-  </si>
-  <si>
-    <t>8th  Vice President of the United States</t>
-  </si>
-  <si>
     <t>Richard Mentor Johnson</t>
   </si>
   <si>
-    <t>William Henry Harrison</t>
-  </si>
-  <si>
-    <t>United States Minister to Colombia   (1828â€“1829)</t>
-  </si>
-  <si>
     <t>Whig</t>
   </si>
   <si>
@@ -142,297 +85,93 @@
     <t>john tyler</t>
   </si>
   <si>
-    <t>10th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>Whig   April 4, 1841  â€“  September 13, 1841</t>
-  </si>
-  <si>
     <t>Office vacant</t>
   </si>
   <si>
-    <t>James K. Polk</t>
-  </si>
-  <si>
-    <t>9th  Governor of Tennessee   (1839â€“1841)</t>
-  </si>
-  <si>
-    <t>George         M. Dallas</t>
-  </si>
-  <si>
-    <t>Zachary Taylor</t>
-  </si>
-  <si>
-    <t>Major General  of the  1st Infantry Regiment   United States Army   (1846â€“1849)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">               Millard Fillmore</t>
-  </si>
-  <si>
     <t>Millard Fillmore</t>
   </si>
   <si>
-    <t>12th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>Franklin Pierce</t>
-  </si>
-  <si>
-    <t>Brigadier General  of the  9th Infantry   United States Army   (1847â€“1848)</t>
-  </si>
-  <si>
     <t>William R. King</t>
   </si>
   <si>
-    <t>James Buchanan</t>
-  </si>
-  <si>
-    <t>United States Minister  to the   Court of St James's   (1853â€“1856)</t>
-  </si>
-  <si>
     <t>John C. Breckinridge</t>
   </si>
   <si>
-    <t>Abraham Lincoln</t>
-  </si>
-  <si>
-    <t>U.S. Representative  for  Illinois' 7th District   (1847â€“1849)</t>
-  </si>
-  <si>
     <t>Hannibal Hamlin</t>
   </si>
   <si>
-    <t>Andrew Johnson</t>
-  </si>
-  <si>
-    <t>16th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>Ulysses S. Grant</t>
-  </si>
-  <si>
-    <t>Commanding General  of the U.S. Army   ( 1864â€“1869 )</t>
-  </si>
-  <si>
     <t>Republican</t>
   </si>
   <si>
     <t>Schuyler Colfax</t>
   </si>
   <si>
-    <t>Rutherford B. Hayes</t>
-  </si>
-  <si>
-    <t>29th &amp; 32nd  Governor of Ohio   (1868â€“1872 &amp; 1876â€“1877)</t>
-  </si>
-  <si>
     <t>William A. Wheeler</t>
   </si>
   <si>
-    <t>James A. Garfield</t>
-  </si>
-  <si>
-    <t>U.S. Representative  for  Ohio's 19th District   (1863â€“1881)</t>
-  </si>
-  <si>
     <t>Chester A. Arthur</t>
   </si>
   <si>
-    <t>20th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>Grover Cleveland</t>
-  </si>
-  <si>
-    <t>28th  Governor of New York   (1883â€“1885)</t>
-  </si>
-  <si>
     <t>Thomas A. Hendricks</t>
   </si>
   <si>
-    <t>Benjamin Harrison</t>
-  </si>
-  <si>
-    <t>U.S. Senator   ( Class 1 )   from  Indiana   (1881â€“1887)</t>
-  </si>
-  <si>
     <t>Levi P. Morton</t>
   </si>
   <si>
-    <t>22nd  President of the United States   (1885â€“1889)</t>
-  </si>
-  <si>
     <t>Adlai Stevenson</t>
   </si>
   <si>
-    <t>William McKinley</t>
-  </si>
-  <si>
-    <t>39th  Governor of Ohio   (1892â€“1896)</t>
-  </si>
-  <si>
     <t>Garret Hobart</t>
   </si>
   <si>
-    <t>Theodore Roosevelt</t>
-  </si>
-  <si>
-    <t>25th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>William Howard Taft</t>
-  </si>
-  <si>
-    <t>42nd  United States Secretary of War   (1904â€“1908)</t>
-  </si>
-  <si>
     <t>James S. Sherman</t>
   </si>
   <si>
-    <t>Woodrow Wilson</t>
-  </si>
-  <si>
-    <t>34th  Governor of New Jersey   (1911â€“1913)</t>
-  </si>
-  <si>
     <t>Thomas R. Marshall</t>
   </si>
   <si>
-    <t>Warren G. Harding</t>
-  </si>
-  <si>
-    <t>U.S. Senator   ( Class 3 )   from  Ohio   (1915â€“1921)</t>
-  </si>
-  <si>
     <t>Calvin Coolidge</t>
   </si>
   <si>
-    <t>29th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>Herbert Hoover</t>
-  </si>
-  <si>
-    <t>3rd  United States Secretary of Commerce   (1921â€“1928)</t>
-  </si>
-  <si>
     <t>Charles Curtis</t>
   </si>
   <si>
-    <t>Franklin D. Roosevelt</t>
-  </si>
-  <si>
-    <t>44th  Governor of New York   ( 1929â€“1932 )</t>
-  </si>
-  <si>
     <t>John Nance Garner</t>
   </si>
   <si>
-    <t>Harry S. Truman</t>
-  </si>
-  <si>
-    <t>34th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>Dwight D. Eisenhower</t>
-  </si>
-  <si>
-    <t>Supreme Allied Commander Europe   ( 1949â€“1952 )</t>
-  </si>
-  <si>
     <t>Richard Nixon</t>
   </si>
   <si>
-    <t>John F. Kennedy</t>
-  </si>
-  <si>
-    <t>U.S. Senator   ( Class 1 )   from  Massachusetts   (1953â€“1960)</t>
-  </si>
-  <si>
     <t>Lyndon B. Johnson</t>
   </si>
   <si>
-    <t>37th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>36th  Vice President of the United States   (1953â€“1961)</t>
-  </si>
-  <si>
     <t>Spiro Agnew</t>
   </si>
   <si>
-    <t>Gerald Ford</t>
-  </si>
-  <si>
-    <t>40th  Vice President of the United States</t>
-  </si>
-  <si>
-    <t>Jimmy Carter</t>
-  </si>
-  <si>
-    <t>76th  Governor of Georgia   (1971â€“1975)</t>
-  </si>
-  <si>
     <t>Walter Mondale</t>
   </si>
   <si>
-    <t>Ronald Reagan</t>
-  </si>
-  <si>
-    <t>33rd  Governor of California   ( 1967â€“1975 )</t>
-  </si>
-  <si>
     <t>George H. W. Bush</t>
   </si>
   <si>
-    <t>43rd  Vice President of the United States</t>
-  </si>
-  <si>
     <t>Dan Quayle</t>
   </si>
   <si>
-    <t>Bill Clinton</t>
-  </si>
-  <si>
-    <t>40th &amp; 42nd  Governor of Arkansas   (1979â€“1981 &amp; 1983â€“1992)</t>
-  </si>
-  <si>
     <t>Al Gore</t>
   </si>
   <si>
-    <t>George W. Bush</t>
-  </si>
-  <si>
-    <t>46th  Governor of Texas   ( 1995â€“2000 )</t>
-  </si>
-  <si>
     <t>Dick Cheney</t>
   </si>
   <si>
-    <t>Barack Obama</t>
-  </si>
-  <si>
-    <t>U.S. Senator   ( Class 3 )   from  Illinois   ( 2005â€“2008 )</t>
-  </si>
-  <si>
     <t>Joe Biden</t>
   </si>
   <si>
-    <t>Donald Trump</t>
-  </si>
-  <si>
-    <t>Chairman of   The Trump Organization   ( 1971â€“present )</t>
-  </si>
-  <si>
     <t>Mike Pence</t>
   </si>
   <si>
     <t>Nonpartisan</t>
   </si>
   <si>
-    <t>Republicans</t>
-  </si>
-  <si>
     <t>Demorcatic</t>
   </si>
   <si>
@@ -443,16 +182,147 @@
   </si>
   <si>
     <t>date updated</t>
+  </si>
+  <si>
+    <t>Aaron Burr</t>
+  </si>
+  <si>
+    <t>George Clinton</t>
+  </si>
+  <si>
+    <t>George M. Dallas</t>
+  </si>
+  <si>
+    <t>george washington</t>
+  </si>
+  <si>
+    <t>thomas jefferson</t>
+  </si>
+  <si>
+    <t>james madison</t>
+  </si>
+  <si>
+    <t>james monroe</t>
+  </si>
+  <si>
+    <t>john quincy adams</t>
+  </si>
+  <si>
+    <t>andrew jackson</t>
+  </si>
+  <si>
+    <t>martin van buren</t>
+  </si>
+  <si>
+    <t>william henry harrison</t>
+  </si>
+  <si>
+    <t>james k. polk</t>
+  </si>
+  <si>
+    <t>zachary taylor</t>
+  </si>
+  <si>
+    <t>millard fillmore</t>
+  </si>
+  <si>
+    <t>franklin pierce</t>
+  </si>
+  <si>
+    <t>james buchanan</t>
+  </si>
+  <si>
+    <t>abraham lincoln</t>
+  </si>
+  <si>
+    <t>andrew johnson</t>
+  </si>
+  <si>
+    <t>ulysses s. grant</t>
+  </si>
+  <si>
+    <t>rutherford b. hayes</t>
+  </si>
+  <si>
+    <t>james a. garfield</t>
+  </si>
+  <si>
+    <t>chester a. arthur</t>
+  </si>
+  <si>
+    <t>grover cleveland</t>
+  </si>
+  <si>
+    <t>benjamin harrison</t>
+  </si>
+  <si>
+    <t>william mckinley</t>
+  </si>
+  <si>
+    <t>theodore roosevelt</t>
+  </si>
+  <si>
+    <t>william howard taft</t>
+  </si>
+  <si>
+    <t>woodrow wilson</t>
+  </si>
+  <si>
+    <t>warren g. harding</t>
+  </si>
+  <si>
+    <t>calvin coolidge</t>
+  </si>
+  <si>
+    <t>herbert hoover</t>
+  </si>
+  <si>
+    <t>franklin d. roosevelt</t>
+  </si>
+  <si>
+    <t>harry s. truman</t>
+  </si>
+  <si>
+    <t>dwight d. eisenhower</t>
+  </si>
+  <si>
+    <t>john f. kennedy</t>
+  </si>
+  <si>
+    <t>lyndon b. johnson</t>
+  </si>
+  <si>
+    <t>richard nixon</t>
+  </si>
+  <si>
+    <t>gerald ford</t>
+  </si>
+  <si>
+    <t>jimmy carter</t>
+  </si>
+  <si>
+    <t>ronald reagan</t>
+  </si>
+  <si>
+    <t>george h. w. bush</t>
+  </si>
+  <si>
+    <t>bill clinton</t>
+  </si>
+  <si>
+    <t>george w. bush</t>
+  </si>
+  <si>
+    <t>barack obama</t>
+  </si>
+  <si>
+    <t>donald trump</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="179" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -936,12 +806,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1001,9 +869,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1041,7 +909,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1147,7 +1015,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1289,7 +1157,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1297,18 +1165,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="23.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="23.52734375" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="7" max="7" width="23.5546875" style="3"/>
+    <col min="6" max="6" width="23.52734375" style="2"/>
+    <col min="7" max="8" width="23.52734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1321,20 +1190,17 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="H1" t="s">
-        <v>136</v>
-      </c>
-      <c r="I1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1342,28 +1208,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" s="4">
+        <v>4</v>
+      </c>
+      <c r="F2" s="2">
         <v>5000</v>
       </c>
+      <c r="G2" s="1">
+        <v>44391</v>
+      </c>
       <c r="H2" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I2" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1371,28 +1234,25 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="4">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2">
         <v>10000</v>
       </c>
+      <c r="G3" s="1">
+        <v>44391</v>
+      </c>
       <c r="H3" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I3" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1400,28 +1260,25 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="4">
+        <v>49</v>
+      </c>
+      <c r="F4" s="2">
         <v>15000</v>
       </c>
+      <c r="G4" s="1">
+        <v>44391</v>
+      </c>
       <c r="H4" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I4" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1429,28 +1286,25 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>17</v>
-      </c>
-      <c r="G5" s="4">
+        <v>50</v>
+      </c>
+      <c r="F5" s="2">
         <v>20000</v>
       </c>
+      <c r="G5" s="1">
+        <v>44391</v>
+      </c>
       <c r="H5" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I5" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1458,28 +1312,25 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="4">
+        <v>9</v>
+      </c>
+      <c r="F6" s="2">
         <v>25000</v>
       </c>
+      <c r="G6" s="1">
+        <v>44391</v>
+      </c>
       <c r="H6" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I6" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1487,28 +1338,25 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="4">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
         <v>30000</v>
       </c>
+      <c r="G7" s="1">
+        <v>44391</v>
+      </c>
       <c r="H7" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I7" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1516,28 +1364,25 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G8" s="4">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2">
         <v>35000</v>
       </c>
+      <c r="G8" s="1">
+        <v>44391</v>
+      </c>
       <c r="H8" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I8" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1545,28 +1390,25 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="4">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2">
         <v>40000</v>
       </c>
+      <c r="G9" s="1">
+        <v>44391</v>
+      </c>
       <c r="H9" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I9" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1574,28 +1416,25 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" t="s">
-        <v>34</v>
-      </c>
-      <c r="G10" s="4">
+        <v>14</v>
+      </c>
+      <c r="F10" s="2">
         <v>45000</v>
       </c>
+      <c r="G10" s="1">
+        <v>44391</v>
+      </c>
       <c r="H10" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I10" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1603,28 +1442,25 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>36</v>
+        <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="4">
+        <v>16</v>
+      </c>
+      <c r="F11" s="2">
         <v>50000</v>
       </c>
+      <c r="G11" s="1">
+        <v>44391</v>
+      </c>
       <c r="H11" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I11" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1632,28 +1468,25 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="E12" t="s">
-        <v>26</v>
-      </c>
-      <c r="F12" t="s">
-        <v>41</v>
-      </c>
-      <c r="G12" s="4">
+        <v>51</v>
+      </c>
+      <c r="F12" s="2">
         <v>55000</v>
       </c>
+      <c r="G12" s="1">
+        <v>44391</v>
+      </c>
       <c r="H12" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I12" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1661,28 +1494,25 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="4">
+        <v>17</v>
+      </c>
+      <c r="F13" s="2">
         <v>60000</v>
       </c>
+      <c r="G13" s="1">
+        <v>44391</v>
+      </c>
       <c r="H13" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I13" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1690,28 +1520,25 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="4">
+        <v>16</v>
+      </c>
+      <c r="F14" s="2">
         <v>65000</v>
       </c>
+      <c r="G14" s="1">
+        <v>44391</v>
+      </c>
       <c r="H14" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I14" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1719,28 +1546,25 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="4">
+        <v>18</v>
+      </c>
+      <c r="F15" s="2">
         <v>75000</v>
       </c>
+      <c r="G15" s="1">
+        <v>44391</v>
+      </c>
       <c r="H15" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I15" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1748,28 +1572,25 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>11</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
-      </c>
-      <c r="F16" t="s">
-        <v>52</v>
-      </c>
-      <c r="G16" s="4">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2">
         <v>85000</v>
       </c>
+      <c r="G16" s="1">
+        <v>44391</v>
+      </c>
       <c r="H16" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I16" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1777,28 +1598,25 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G17" s="4">
+        <v>20</v>
+      </c>
+      <c r="F17" s="2">
         <v>95000</v>
       </c>
+      <c r="G17" s="1">
+        <v>44391</v>
+      </c>
       <c r="H17" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I17" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1806,28 +1624,25 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="4">
+        <v>16</v>
+      </c>
+      <c r="F18" s="2">
         <v>105000</v>
       </c>
+      <c r="G18" s="1">
+        <v>44391</v>
+      </c>
       <c r="H18" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I18" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1835,28 +1650,25 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="4">
+        <v>22</v>
+      </c>
+      <c r="F19" s="2">
         <v>115000</v>
       </c>
+      <c r="G19" s="1">
+        <v>44391</v>
+      </c>
       <c r="H19" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I19" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1864,28 +1676,25 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>63</v>
+        <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" t="s">
-        <v>64</v>
-      </c>
-      <c r="G20" s="4">
+        <v>23</v>
+      </c>
+      <c r="F20" s="2">
         <v>125000</v>
       </c>
+      <c r="G20" s="1">
+        <v>44391</v>
+      </c>
       <c r="H20" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I20" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1893,28 +1702,25 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D21" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
-      </c>
-      <c r="G21" s="4">
+        <v>24</v>
+      </c>
+      <c r="F21" s="2">
         <v>135000</v>
       </c>
+      <c r="G21" s="1">
+        <v>44391</v>
+      </c>
       <c r="H21" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I21" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1922,28 +1728,25 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="4">
+        <v>16</v>
+      </c>
+      <c r="F22" s="2">
         <v>145000</v>
       </c>
+      <c r="G22" s="1">
+        <v>44391</v>
+      </c>
       <c r="H22" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I22" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A23">
         <v>21</v>
       </c>
@@ -1951,28 +1754,25 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" s="4">
+        <v>25</v>
+      </c>
+      <c r="F23" s="2">
         <v>155000</v>
       </c>
+      <c r="G23" s="1">
+        <v>44391</v>
+      </c>
       <c r="H23" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I23" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A24">
         <v>22</v>
       </c>
@@ -1983,25 +1783,22 @@
         <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" t="s">
-        <v>74</v>
-      </c>
-      <c r="G24" s="4">
+        <v>26</v>
+      </c>
+      <c r="F24" s="2">
         <v>165000</v>
       </c>
+      <c r="G24" s="1">
+        <v>44391</v>
+      </c>
       <c r="H24" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I24" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2009,28 +1806,25 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
-        <v>75</v>
+        <v>11</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" t="s">
-        <v>76</v>
-      </c>
-      <c r="G25" s="4">
+        <v>27</v>
+      </c>
+      <c r="F25" s="2">
         <v>175000</v>
       </c>
+      <c r="G25" s="1">
+        <v>44391</v>
+      </c>
       <c r="H25" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I25" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2038,28 +1832,25 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F26" t="s">
-        <v>79</v>
-      </c>
-      <c r="G26" s="4">
+        <v>28</v>
+      </c>
+      <c r="F26" s="2">
         <v>185000</v>
       </c>
+      <c r="G26" s="1">
+        <v>44391</v>
+      </c>
       <c r="H26" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I26" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2067,28 +1858,25 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D27" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F27" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27" s="4">
+        <v>16</v>
+      </c>
+      <c r="F27" s="2">
         <v>195000</v>
       </c>
+      <c r="G27" s="1">
+        <v>44391</v>
+      </c>
       <c r="H27" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I27" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2096,28 +1884,25 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>60</v>
-      </c>
-      <c r="F28" t="s">
-        <v>84</v>
-      </c>
-      <c r="G28" s="4">
+        <v>29</v>
+      </c>
+      <c r="F28" s="2">
         <v>205000</v>
       </c>
+      <c r="G28" s="1">
+        <v>44391</v>
+      </c>
       <c r="H28" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I28" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2125,28 +1910,25 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>86</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" s="4">
+        <v>30</v>
+      </c>
+      <c r="F29" s="2">
         <v>225000</v>
       </c>
+      <c r="G29" s="1">
+        <v>44391</v>
+      </c>
       <c r="H29" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I29" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A30">
         <v>27</v>
       </c>
@@ -2154,28 +1936,25 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>133</v>
-      </c>
-      <c r="F30" t="s">
-        <v>87</v>
-      </c>
-      <c r="G30" s="4">
+        <v>30</v>
+      </c>
+      <c r="F30" s="2">
         <v>225000</v>
       </c>
+      <c r="G30" s="1">
+        <v>44391</v>
+      </c>
       <c r="H30" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I30" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A31">
         <v>28</v>
       </c>
@@ -2183,28 +1962,25 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>60</v>
-      </c>
-      <c r="F31" t="s">
-        <v>90</v>
-      </c>
-      <c r="G31" s="4">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2">
         <v>235000</v>
       </c>
+      <c r="G31" s="1">
+        <v>44391</v>
+      </c>
       <c r="H31" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I31" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A32">
         <v>29</v>
       </c>
@@ -2212,28 +1988,25 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="D32" t="s">
-        <v>91</v>
+        <v>21</v>
       </c>
       <c r="E32" t="s">
-        <v>60</v>
-      </c>
-      <c r="F32" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" s="4">
+        <v>16</v>
+      </c>
+      <c r="F32" s="2">
         <v>245000</v>
       </c>
+      <c r="G32" s="1">
+        <v>44391</v>
+      </c>
       <c r="H32" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I32" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A33">
         <v>30</v>
       </c>
@@ -2241,28 +2014,25 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>60</v>
-      </c>
-      <c r="F33" t="s">
-        <v>94</v>
-      </c>
-      <c r="G33" s="4">
+        <v>32</v>
+      </c>
+      <c r="F33" s="2">
         <v>255000</v>
       </c>
+      <c r="G33" s="1">
+        <v>44391</v>
+      </c>
       <c r="H33" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I33" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A34">
         <v>31</v>
       </c>
@@ -2270,28 +2040,25 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D34" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="E34" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34" s="4">
+        <v>33</v>
+      </c>
+      <c r="F34" s="2">
         <v>265000</v>
       </c>
+      <c r="G34" s="1">
+        <v>44391</v>
+      </c>
       <c r="H34" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I34" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A35">
         <v>32</v>
       </c>
@@ -2299,28 +2066,25 @@
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>11</v>
       </c>
       <c r="E35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="4">
+        <v>16</v>
+      </c>
+      <c r="F35" s="2">
         <v>275000</v>
       </c>
+      <c r="G35" s="1">
+        <v>44391</v>
+      </c>
       <c r="H35" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I35" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A36">
         <v>33</v>
       </c>
@@ -2328,28 +2092,25 @@
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>21</v>
       </c>
       <c r="E36" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" t="s">
-        <v>102</v>
-      </c>
-      <c r="G36" s="4">
+        <v>34</v>
+      </c>
+      <c r="F36" s="2">
         <v>285000</v>
       </c>
+      <c r="G36" s="1">
+        <v>44391</v>
+      </c>
       <c r="H36" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I36" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A37">
         <v>34</v>
       </c>
@@ -2357,28 +2118,25 @@
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>11</v>
       </c>
       <c r="E37" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" t="s">
-        <v>105</v>
-      </c>
-      <c r="G37" s="4">
+        <v>35</v>
+      </c>
+      <c r="F37" s="2">
         <v>295000</v>
       </c>
+      <c r="G37" s="1">
+        <v>44391</v>
+      </c>
       <c r="H37" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I37" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A38">
         <v>35</v>
       </c>
@@ -2386,28 +2144,25 @@
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>11</v>
       </c>
       <c r="E38" t="s">
-        <v>26</v>
-      </c>
-      <c r="F38" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="4">
+        <v>16</v>
+      </c>
+      <c r="F38" s="2">
         <v>305000</v>
       </c>
+      <c r="G38" s="1">
+        <v>44391</v>
+      </c>
       <c r="H38" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I38" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A39">
         <v>36</v>
       </c>
@@ -2415,28 +2170,25 @@
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="D39" t="s">
-        <v>107</v>
+        <v>21</v>
       </c>
       <c r="E39" t="s">
-        <v>60</v>
-      </c>
-      <c r="F39" t="s">
-        <v>108</v>
-      </c>
-      <c r="G39" s="4">
+        <v>36</v>
+      </c>
+      <c r="F39" s="2">
         <v>315000</v>
       </c>
+      <c r="G39" s="1">
+        <v>44391</v>
+      </c>
       <c r="H39" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I39" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A40">
         <v>37</v>
       </c>
@@ -2444,28 +2196,25 @@
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="D40" t="s">
-        <v>110</v>
+        <v>21</v>
       </c>
       <c r="E40" t="s">
-        <v>60</v>
-      </c>
-      <c r="F40" t="s">
-        <v>38</v>
-      </c>
-      <c r="G40" s="4">
+        <v>16</v>
+      </c>
+      <c r="F40" s="2">
         <v>325000</v>
       </c>
+      <c r="G40" s="1">
+        <v>44391</v>
+      </c>
       <c r="H40" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I40" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A41">
         <v>38</v>
       </c>
@@ -2473,28 +2222,25 @@
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D41" t="s">
-        <v>112</v>
+        <v>11</v>
       </c>
       <c r="E41" t="s">
-        <v>26</v>
-      </c>
-      <c r="F41" t="s">
-        <v>113</v>
-      </c>
-      <c r="G41" s="4">
+        <v>37</v>
+      </c>
+      <c r="F41" s="2">
         <v>335000</v>
       </c>
+      <c r="G41" s="1">
+        <v>44391</v>
+      </c>
       <c r="H41" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I41" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A42">
         <v>39</v>
       </c>
@@ -2502,28 +2248,25 @@
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>114</v>
+        <v>88</v>
       </c>
       <c r="D42" t="s">
-        <v>115</v>
+        <v>21</v>
       </c>
       <c r="E42" t="s">
-        <v>60</v>
-      </c>
-      <c r="F42" t="s">
-        <v>116</v>
-      </c>
-      <c r="G42" s="4">
+        <v>38</v>
+      </c>
+      <c r="F42" s="2">
         <v>345000</v>
       </c>
+      <c r="G42" s="1">
+        <v>44391</v>
+      </c>
       <c r="H42" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I42" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A43">
         <v>40</v>
       </c>
@@ -2531,28 +2274,25 @@
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="D43" t="s">
-        <v>117</v>
+        <v>21</v>
       </c>
       <c r="E43" t="s">
-        <v>60</v>
-      </c>
-      <c r="F43" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" s="4">
+        <v>39</v>
+      </c>
+      <c r="F43" s="2">
         <v>355000</v>
       </c>
+      <c r="G43" s="1">
+        <v>44391</v>
+      </c>
       <c r="H43" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I43" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A44">
         <v>41</v>
       </c>
@@ -2560,28 +2300,25 @@
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>90</v>
       </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="E44" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" t="s">
-        <v>121</v>
-      </c>
-      <c r="G44" s="4">
+        <v>40</v>
+      </c>
+      <c r="F44" s="2">
         <v>365000</v>
       </c>
+      <c r="G44" s="1">
+        <v>44391</v>
+      </c>
       <c r="H44" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I44" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A45">
         <v>42</v>
       </c>
@@ -2589,28 +2326,25 @@
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="D45" t="s">
-        <v>123</v>
+        <v>21</v>
       </c>
       <c r="E45" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" t="s">
-        <v>124</v>
-      </c>
-      <c r="G45" s="4">
+        <v>41</v>
+      </c>
+      <c r="F45" s="2">
         <v>375000</v>
       </c>
+      <c r="G45" s="1">
+        <v>44391</v>
+      </c>
       <c r="H45" s="1">
-        <v>44391</v>
-      </c>
-      <c r="I45" s="1">
-        <v>40972</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+        <v>40972</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A46">
         <v>43</v>
       </c>
@@ -2618,28 +2352,25 @@
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>11</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" t="s">
-        <v>127</v>
-      </c>
-      <c r="G46" s="4">
+        <v>42</v>
+      </c>
+      <c r="F46" s="2">
         <v>395000</v>
       </c>
-      <c r="H46" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I46" s="2">
+      <c r="G46" s="1">
+        <v>44391</v>
+      </c>
+      <c r="H46" s="1">
         <v>43862</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A47">
         <v>43</v>
       </c>
@@ -2647,28 +2378,25 @@
         <v>44</v>
       </c>
       <c r="C47" t="s">
-        <v>125</v>
+        <v>92</v>
       </c>
       <c r="D47" t="s">
-        <v>126</v>
+        <v>11</v>
       </c>
       <c r="E47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" t="s">
-        <v>127</v>
-      </c>
-      <c r="G47" s="4">
+        <v>42</v>
+      </c>
+      <c r="F47" s="2">
         <v>395000</v>
       </c>
-      <c r="H47" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I47" s="2">
+      <c r="G47" s="1">
+        <v>44391</v>
+      </c>
+      <c r="H47" s="1">
         <v>43862</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.5">
       <c r="A48">
         <v>44</v>
       </c>
@@ -2676,28 +2404,26 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="D48" t="s">
-        <v>129</v>
+        <v>21</v>
       </c>
       <c r="E48" t="s">
-        <v>132</v>
-      </c>
-      <c r="F48" t="s">
-        <v>130</v>
-      </c>
-      <c r="G48" s="4">
+        <v>43</v>
+      </c>
+      <c r="F48" s="2">
         <v>405000</v>
       </c>
-      <c r="H48" s="2">
-        <v>44391</v>
-      </c>
-      <c r="I48" s="2">
+      <c r="G48" s="1">
+        <v>44391</v>
+      </c>
+      <c r="H48" s="1">
         <v>43862</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H48" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <dataConsolidate/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>